<commit_message>
EPBDS-10027 SpreadsheetResult field naming is inconsistent with Datatype and input arguments for non-ASCII symbols
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_SPR_model_naming_verification.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_SPR_model_naming_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC8E328-68B1-426E-9073-4433000642C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0749D389-B2E4-4436-BDB8-30E6BAF38082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="143" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="143" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,27 +636,15 @@
     <t>_res_.$Step2["aaa"]</t>
   </si>
   <si>
-    <t>_res_.$Step2["tiest"]:Integer</t>
-  </si>
-  <si>
     <t>_res_.$Step2["aaa"]:Integer</t>
   </si>
   <si>
-    <t>_res_.$Step2["asutarisuku"]:Integer</t>
-  </si>
-  <si>
     <t>_res_.$Step2["asutarisuku"]</t>
   </si>
   <si>
-    <t>_res_.$Step2["TestYYY"]:Integer</t>
-  </si>
-  <si>
     <t>_res_.$Step2["TestYYY"]</t>
   </si>
   <si>
-    <t>_res_.$Step2["Yin_Shua_Zhong_De_Xing_Hao_"]:Integer</t>
-  </si>
-  <si>
     <t>_res_.$Step2["Yin_Shua_Zhong_De_Xing_Hao_"]</t>
   </si>
   <si>
@@ -757,6 +745,18 @@
   </si>
   <si>
     <t>Result0</t>
+  </si>
+  <si>
+    <t>_res_.$Step2["тест"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step2["アスタリスク"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step2["TestЫЫЫ"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step2["印刷中的星号"]:Integer</t>
   </si>
 </sst>
 </file>
@@ -1393,27 +1393,27 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.86328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.59765625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.265625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.86328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.73046875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="24" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.73046875" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="2:10" s="5" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" s="5" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="41" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>46</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="40" t="s">
         <v>27</v>
       </c>
@@ -1511,7 +1511,7 @@
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="16" t="s">
         <v>0</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="14" t="s">
         <v>108</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="14" t="s">
         <v>109</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="16" t="s">
         <v>44</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="14" t="s">
         <v>110</v>
       </c>
@@ -1584,13 +1584,13 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="G20" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="40" t="s">
         <v>78</v>
       </c>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="G22" s="40"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="16" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="16" t="s">
         <v>2</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" s="16" t="s">
         <v>5</v>
       </c>
@@ -1642,14 +1642,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B30" s="40" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="16" t="s">
         <v>19</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B32" s="16" t="s">
         <v>19</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B33" s="11" t="s">
         <v>31</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B36" s="40" t="s">
         <v>36</v>
       </c>
@@ -1693,7 +1693,7 @@
       <c r="G36" s="40"/>
       <c r="H36" s="40"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B37" s="16" t="s">
         <v>39</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B39" s="16" t="s">
         <v>39</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B40" s="11">
         <v>1</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B44" s="40" t="s">
         <v>81</v>
       </c>
@@ -1782,7 +1782,7 @@
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B45" s="16" t="s">
         <v>37</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B46" s="16" t="s">
         <v>38</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B48" s="11">
         <v>1</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="F48" s="11"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B52" s="40" t="s">
         <v>80</v>
       </c>
@@ -1851,7 +1851,7 @@
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B53" s="16" t="s">
         <v>37</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B54" s="16" t="s">
         <v>38</v>
       </c>
@@ -1879,7 +1879,7 @@
       <c r="E54" s="16"/>
       <c r="F54" s="16"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B55" s="16" t="s">
         <v>37</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B56" s="11">
         <v>1</v>
       </c>
@@ -1936,25 +1936,25 @@
       <selection activeCell="B52" sqref="B52:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.86328125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="41" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.3984375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.265625" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="36.3984375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.59765625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.86328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B4" s="43" t="s">
         <v>54</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B5" s="16" t="s">
         <v>57</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B6" s="16" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B7" s="14" t="s">
         <v>112</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B8" s="14" t="s">
         <v>113</v>
       </c>
@@ -2040,17 +2040,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B11" s="50" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="50"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B12" s="16" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
         <v>2</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B16" s="41" t="s">
         <v>65</v>
       </c>
@@ -2084,7 +2084,7 @@
       <c r="F16" s="49"/>
       <c r="G16" s="42"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B17" s="16" t="s">
         <v>66</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B18" s="16" t="s">
         <v>66</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B19" s="11" t="s">
         <v>59</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
@@ -2156,17 +2156,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:9" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:9" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B30" s="43" t="s">
         <v>71</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="H30" s="42"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B31" s="16" t="s">
         <v>57</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B32" s="16" t="s">
         <v>0</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B33" s="14" t="s">
         <v>112</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" s="14" t="s">
         <v>113</v>
       </c>
@@ -2257,12 +2257,12 @@
       <c r="I34" s="8"/>
       <c r="J34" s="9"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="47" t="s">
         <v>73</v>
       </c>
@@ -2271,7 +2271,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="16" t="s">
         <v>0</v>
       </c>
@@ -2282,7 +2282,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="16" t="s">
         <v>2</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="16" t="s">
         <v>5</v>
       </c>
@@ -2304,7 +2304,7 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="40" t="s">
         <v>75</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="H43" s="40"/>
       <c r="I43" s="40"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="16" t="s">
         <v>66</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="16" t="s">
         <v>66</v>
       </c>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B46" s="11" t="s">
         <v>59</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B47" s="11" t="s">
         <v>60</v>
       </c>
@@ -2409,22 +2409,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="49" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="50" spans="2:7" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B50" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B52" s="40" t="s">
         <v>95</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
     </row>
-    <row r="53" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B53" s="16" t="s">
         <v>57</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B54" s="16" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B55" s="14" t="s">
         <v>112</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B56" s="14" t="s">
         <v>113</v>
       </c>
@@ -2468,19 +2468,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B57" s="20"/>
       <c r="C57" s="21"/>
       <c r="D57" s="21"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B58" s="40" t="s">
         <v>97</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="19"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B59" s="16" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D59" s="22"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B60" s="16" t="s">
         <v>2</v>
       </c>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B61" s="16" t="s">
         <v>5</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="D61" s="6"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B64" s="40" t="s">
         <v>100</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F64" s="40"/>
       <c r="G64" s="40"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B65" s="16" t="s">
         <v>66</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B66" s="16" t="s">
         <v>66</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B67" s="11" t="s">
         <v>60</v>
       </c>
@@ -2573,14 +2573,14 @@
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B70" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C70" s="40"/>
       <c r="D70" s="40"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B71" s="16" t="s">
         <v>57</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B72" s="16" t="s">
         <v>0</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B73" s="14" t="s">
         <v>112</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B74" s="16" t="s">
         <v>5</v>
       </c>
@@ -2624,14 +2624,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B76" s="40" t="s">
         <v>99</v>
       </c>
       <c r="C76" s="40"/>
       <c r="D76" s="19"/>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B77" s="16" t="s">
         <v>0</v>
       </c>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B78" s="16" t="s">
         <v>2</v>
       </c>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B79" s="16" t="s">
         <v>5</v>
       </c>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="D79" s="6"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B82" s="40" t="s">
         <v>102</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="G82" s="40"/>
       <c r="H82" s="23"/>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B83" s="16" t="s">
         <v>66</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B84" s="16" t="s">
         <v>66</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B85" s="11" t="s">
         <v>60</v>
       </c>
@@ -2759,27 +2759,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.3984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="25.59765625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.73046875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="28" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.3984375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="44" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="53" t="s">
         <v>117</v>
       </c>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="G4" s="52"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="33" t="s">
         <v>118</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="31" t="s">
         <v>5</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="31" t="s">
         <v>121</v>
       </c>
@@ -2839,33 +2839,33 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B9" s="6"/>
       <c r="C9" s="26"/>
     </row>
-    <row r="10" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B10" s="53" t="s">
         <v>170</v>
       </c>
       <c r="C10" s="54"/>
     </row>
-    <row r="11" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B12" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B13" s="23">
         <v>1</v>
       </c>
@@ -2873,19 +2873,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B14" s="6"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B15" s="6"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="53" t="s">
         <v>123</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="G17" s="54"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="31" t="s">
         <v>0</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="31" t="s">
         <v>2</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="31" t="s">
         <v>5</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="31" t="s">
         <v>121</v>
       </c>
@@ -2945,8 +2945,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="52" t="s">
         <v>171</v>
       </c>
@@ -2954,7 +2954,7 @@
       <c r="D24" s="52"/>
       <c r="E24" s="52"/>
     </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B25" s="31" t="s">
         <v>37</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B26" s="31" t="s">
         <v>37</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B27" s="23">
         <v>1</v>
       </c>
@@ -2996,15 +2996,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B33" s="51" t="s">
         <v>126</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B34" s="23" t="s">
         <v>127</v>
       </c>
@@ -3025,10 +3025,10 @@
         <v>128</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B35" s="23" t="s">
         <v>2</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B36" s="23" t="s">
         <v>5</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B37" s="23" t="s">
         <v>121</v>
       </c>
@@ -3061,15 +3061,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B41" s="52" t="s">
         <v>168</v>
       </c>
       <c r="C41" s="52"/>
     </row>
-    <row r="42" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B42" s="31" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B43" s="31" t="s">
         <v>2</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B44" s="31" t="s">
         <v>5</v>
       </c>
@@ -3093,9 +3093,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B47" s="52" t="s">
         <v>197</v>
       </c>
@@ -3106,7 +3106,7 @@
       <c r="G47" s="52"/>
       <c r="H47" s="52"/>
     </row>
-    <row r="48" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B48" s="31" t="s">
         <v>37</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B49" s="31" t="s">
         <v>37</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B50" s="23">
         <v>1</v>
       </c>
@@ -3173,18 +3173,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="55" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B55" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B57" s="51" t="s">
         <v>132</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B58" s="31" t="s">
         <v>0</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B59" s="31" t="s">
         <v>2</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B60" s="31" t="s">
         <v>5</v>
       </c>
@@ -3236,7 +3236,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B61" s="31" t="s">
         <v>121</v>
       </c>
@@ -3250,18 +3250,18 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B63" s="52" t="s">
         <v>190</v>
       </c>
       <c r="C63" s="52"/>
     </row>
-    <row r="64" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B64" s="31" t="s">
         <v>0</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B65" s="31" t="s">
         <v>2</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B66" s="31" t="s">
         <v>5</v>
       </c>
@@ -3285,8 +3285,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B68" s="52" t="s">
         <v>196</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="G68" s="52"/>
       <c r="H68" s="52"/>
     </row>
-    <row r="69" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B69" s="31" t="s">
         <v>37</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B70" s="31" t="s">
         <v>37</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="71" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B71" s="23">
         <v>1</v>
       </c>
@@ -3366,29 +3366,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B74" s="51" t="s">
         <v>142</v>
       </c>
       <c r="C74" s="51"/>
       <c r="D74" s="51"/>
       <c r="F74" s="51" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G74" s="51"/>
       <c r="H74" s="51"/>
     </row>
-    <row r="75" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B75" s="31" t="s">
         <v>143</v>
       </c>
@@ -3402,13 +3402,13 @@
         <v>143</v>
       </c>
       <c r="G75" s="33" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H75" s="33" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B76" s="33" t="s">
         <v>112</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B77" s="33" t="s">
         <v>113</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B78" s="33" t="s">
         <v>147</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B79" s="33" t="s">
         <v>149</v>
       </c>
@@ -3465,14 +3465,14 @@
         <v>150</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G79" s="24"/>
       <c r="H79" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B80" s="33" t="s">
         <v>151</v>
       </c>
@@ -3481,14 +3481,14 @@
         <v>152</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G80" s="24"/>
       <c r="H80" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B81" s="31" t="s">
         <v>153</v>
       </c>
@@ -3497,14 +3497,14 @@
         <v>146</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G81" s="24"/>
       <c r="H81" s="24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B82" s="31" t="s">
         <v>154</v>
       </c>
@@ -3513,14 +3513,14 @@
         <v>129</v>
       </c>
       <c r="F82" s="33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G82" s="24"/>
       <c r="H82" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B83" s="31" t="s">
         <v>155</v>
       </c>
@@ -3529,14 +3529,14 @@
         <v>148</v>
       </c>
       <c r="F83" s="33" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G83" s="24"/>
       <c r="H83" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B84" s="31" t="s">
         <v>156</v>
       </c>
@@ -3545,14 +3545,14 @@
         <v>150</v>
       </c>
       <c r="F84" s="33" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G84" s="24"/>
       <c r="H84" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B85" s="31" t="s">
         <v>157</v>
       </c>
@@ -3561,28 +3561,28 @@
         <v>152</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G85" s="24"/>
       <c r="H85" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B86" s="28"/>
       <c r="F86" s="28"/>
     </row>
-    <row r="87" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B87" s="52" t="s">
         <v>193</v>
       </c>
       <c r="C87" s="52"/>
       <c r="F87" s="52" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G87" s="52"/>
     </row>
-    <row r="88" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B88" s="31" t="s">
         <v>0</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B89" s="31" t="s">
         <v>2</v>
       </c>
@@ -3607,10 +3607,10 @@
         <v>2</v>
       </c>
       <c r="G89" s="24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B90" s="31" t="s">
         <v>5</v>
       </c>
@@ -3624,35 +3624,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B91" s="31" t="s">
         <v>121</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F91" s="31" t="s">
         <v>121</v>
       </c>
       <c r="G91" s="24" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B92" s="28"/>
       <c r="F92" s="28"/>
     </row>
-    <row r="93" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B93" s="52" t="s">
         <v>195</v>
       </c>
       <c r="C93" s="52"/>
       <c r="F93" s="52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G93" s="52"/>
     </row>
-    <row r="94" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B94" s="31" t="s">
         <v>37</v>
       </c>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="H94" s="27"/>
     </row>
-    <row r="95" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B95" s="31" t="s">
         <v>37</v>
       </c>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="H95" s="27"/>
     </row>
-    <row r="96" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B96" s="23">
         <v>1</v>
       </c>
@@ -3700,25 +3700,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B97" s="28"/>
       <c r="F97" s="6"/>
       <c r="G97" s="26"/>
       <c r="H97" s="26"/>
     </row>
-    <row r="98" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B98" s="28"/>
       <c r="F98" s="6"/>
       <c r="G98" s="26"/>
       <c r="H98" s="26"/>
     </row>
-    <row r="99" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B99" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B101" s="51" t="s">
         <v>134</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B102" s="38" t="s">
         <v>135</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B103" s="33" t="s">
         <v>137</v>
       </c>
@@ -3749,7 +3749,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B104" s="33" t="s">
         <v>138</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B105" s="33" t="s">
         <v>139</v>
       </c>
@@ -3771,7 +3771,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B106" s="33" t="s">
         <v>140</v>
       </c>
@@ -3782,7 +3782,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B107" s="33" t="s">
         <v>141</v>
       </c>
@@ -3793,18 +3793,18 @@
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B109" s="52" t="s">
         <v>199</v>
       </c>
       <c r="C109" s="52"/>
     </row>
-    <row r="110" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B110" s="31" t="s">
         <v>0</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B111" s="31" t="s">
         <v>2</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="112" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B112" s="31" t="s">
         <v>5</v>
       </c>
@@ -3828,9 +3828,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="114" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B115" s="52" t="s">
         <v>201</v>
       </c>
@@ -3840,27 +3840,27 @@
       <c r="F115" s="52"/>
       <c r="G115" s="52"/>
     </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B116" s="31" t="s">
         <v>37</v>
       </c>
       <c r="C116" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="D116" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="D116" s="32" t="s">
-        <v>205</v>
-      </c>
       <c r="E116" s="32" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="F116" s="32" t="s">
-        <v>208</v>
+        <v>243</v>
       </c>
       <c r="G116" s="32" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B117" s="31" t="s">
         <v>37</v>
       </c>
@@ -3871,16 +3871,16 @@
         <v>203</v>
       </c>
       <c r="E117" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="F117" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="G117" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="F117" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="G117" s="32" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B118" s="23">
         <v>1</v>
       </c>
@@ -3900,19 +3900,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="121" spans="2:12" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B121" s="29" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="122" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="123" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B123" s="51" t="s">
         <v>158</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="K123" s="51"/>
       <c r="L123" s="51"/>
     </row>
-    <row r="124" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B124" s="31" t="s">
         <v>143</v>
       </c>
@@ -3962,18 +3962,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="125" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B125" s="23" t="s">
         <v>159</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D125" s="24" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E125" s="24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F125" s="24" t="s">
         <v>150</v>
@@ -3997,14 +3997,14 @@
         <v>152</v>
       </c>
     </row>
-    <row r="127" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="128" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B128" s="52" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C128" s="52"/>
     </row>
-    <row r="129" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B129" s="31" t="s">
         <v>0</v>
       </c>
@@ -4012,15 +4012,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B130" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B131" s="31" t="s">
         <v>5</v>
       </c>
@@ -4028,11 +4028,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="133" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="134" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B134" s="52" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C134" s="52"/>
       <c r="D134" s="52"/>
@@ -4040,7 +4040,7 @@
       <c r="F134" s="52"/>
       <c r="G134" s="52"/>
     </row>
-    <row r="135" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B135" s="31" t="s">
         <v>37</v>
       </c>
@@ -4054,13 +4054,13 @@
         <v>178</v>
       </c>
       <c r="F135" s="32" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B136" s="31" t="s">
         <v>37</v>
       </c>
@@ -4074,13 +4074,13 @@
         <v>175</v>
       </c>
       <c r="F136" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B137" s="23">
         <v>1</v>
       </c>
@@ -4098,12 +4098,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="139" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="140" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="141" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="142" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B144" s="51" t="s">
         <v>160</v>
       </c>
@@ -4111,7 +4111,7 @@
       <c r="D144" s="51"/>
       <c r="E144" s="51"/>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B145" s="31" t="s">
         <v>0</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B146" s="31" t="s">
         <v>2</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B147" s="31" t="s">
         <v>5</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B148" s="31" t="s">
         <v>121</v>
       </c>
@@ -4167,21 +4167,21 @@
         <v>122</v>
       </c>
     </row>
-    <row r="149" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B149" s="6"/>
       <c r="C149" s="26"/>
       <c r="D149" s="26"/>
       <c r="E149" s="26"/>
     </row>
-    <row r="150" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B150" s="52" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C150" s="52"/>
       <c r="D150" s="26"/>
       <c r="E150" s="26"/>
     </row>
-    <row r="151" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B151" s="31" t="s">
         <v>0</v>
       </c>
@@ -4191,17 +4191,17 @@
       <c r="D151" s="26"/>
       <c r="E151" s="26"/>
     </row>
-    <row r="152" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B152" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D152" s="26"/>
       <c r="E152" s="26"/>
     </row>
-    <row r="153" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B153" s="31" t="s">
         <v>5</v>
       </c>
@@ -4211,21 +4211,21 @@
       <c r="D153" s="26"/>
       <c r="E153" s="26"/>
     </row>
-    <row r="154" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B154" s="6"/>
       <c r="C154" s="26"/>
       <c r="D154" s="26"/>
       <c r="E154" s="26"/>
     </row>
-    <row r="155" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B155" s="52" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C155" s="52"/>
       <c r="D155" s="52"/>
       <c r="E155" s="52"/>
     </row>
-    <row r="156" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B156" s="31" t="s">
         <v>37</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="157" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B157" s="31" t="s">
         <v>37</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="158" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B158" s="23">
         <v>1</v>
       </c>
@@ -4267,19 +4267,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B159" s="6"/>
       <c r="C159" s="26"/>
       <c r="D159" s="26"/>
       <c r="E159" s="26"/>
     </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
       <c r="E160" s="5"/>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B161" s="51" t="s">
         <v>163</v>
       </c>
@@ -4287,7 +4287,7 @@
       <c r="D161" s="51"/>
       <c r="E161" s="51"/>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B162" s="31" t="s">
         <v>0</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B163" s="33" t="s">
         <v>112</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B164" s="31" t="s">
         <v>5</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B165" s="33" t="s">
         <v>147</v>
       </c>
@@ -4343,15 +4343,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B168" s="52" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C168" s="52"/>
       <c r="D168" s="26"/>
       <c r="E168" s="26"/>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B169" s="31" t="s">
         <v>0</v>
       </c>
@@ -4361,17 +4361,17 @@
       <c r="D169" s="26"/>
       <c r="E169" s="26"/>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B170" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D170" s="26"/>
       <c r="E170" s="26"/>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B171" s="31" t="s">
         <v>5</v>
       </c>
@@ -4381,21 +4381,21 @@
       <c r="D171" s="26"/>
       <c r="E171" s="26"/>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B172" s="6"/>
       <c r="C172" s="26"/>
       <c r="D172" s="26"/>
       <c r="E172" s="26"/>
     </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B173" s="52" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C173" s="52"/>
       <c r="D173" s="52"/>
       <c r="E173" s="52"/>
     </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B174" s="36" t="s">
         <v>37</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B175" s="36" t="s">
         <v>37</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B176" s="34">
         <v>1</v>
       </c>

</xml_diff>